<commit_message>
check spelling or synonymn for species added
</commit_message>
<xml_diff>
--- a/inst/extdata/DARWIN_CORE_HERBARIUM_RECORDS_TEMPLATE.xlsx
+++ b/inst/extdata/DARWIN_CORE_HERBARIUM_RECORDS_TEMPLATE.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="17916" windowHeight="9493" tabRatio="198"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17916" windowHeight="9492" tabRatio="198"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="165">
   <si>
     <t>GLOBAL_UNIQUE_IDENTIFIER</t>
   </si>
@@ -191,342 +190,359 @@
     <t>candida</t>
   </si>
   <si>
+    <t>HONG KONG</t>
+  </si>
+  <si>
+    <t>New Territories</t>
+  </si>
+  <si>
+    <t>Sai Kung District</t>
+  </si>
+  <si>
+    <t>Yung Shue O</t>
+  </si>
+  <si>
+    <t>FLORA OF CHINA</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Liana.</t>
+  </si>
+  <si>
+    <t>in dense forest.</t>
+  </si>
+  <si>
+    <t>CABINET_1_1</t>
+  </si>
+  <si>
+    <t>in herbarium</t>
+  </si>
+  <si>
+    <t>GPS</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>50m</t>
+  </si>
+  <si>
+    <t>2015-02-04</t>
+  </si>
+  <si>
+    <t>JL0020</t>
+  </si>
+  <si>
+    <t>MALVACEAE</t>
+  </si>
+  <si>
+    <t>Swartzia</t>
+  </si>
+  <si>
+    <t>australis</t>
+  </si>
+  <si>
+    <t>herb, 10-15cm.</t>
+  </si>
+  <si>
+    <t>Sea shore, along the sea shore, near the mangroves. Grow in open areas.</t>
+  </si>
+  <si>
+    <t>CABINET_1_14</t>
+  </si>
+  <si>
+    <t>flowering</t>
+  </si>
+  <si>
+    <t>JL0021</t>
+  </si>
+  <si>
+    <t>COMBRETACEAE</t>
+  </si>
+  <si>
+    <t>Lumnitzera</t>
+  </si>
+  <si>
+    <t>racemosa</t>
+  </si>
+  <si>
+    <t>shrub, 2m tall. Flowers white.</t>
+  </si>
+  <si>
+    <t>Sea shore, along the sea shore, within the mangroves. Not common. Growth with Kandelia candel,Bruguiera gymnorrhiza,Avicennia marina.</t>
+  </si>
+  <si>
+    <t>CABINET_1_16</t>
+  </si>
+  <si>
+    <t>JL0022</t>
+  </si>
+  <si>
+    <t>2014-8-15</t>
+  </si>
+  <si>
+    <t>PASSIFLORACEAE</t>
+  </si>
+  <si>
+    <t>Cyclobalanosis</t>
+  </si>
+  <si>
+    <t>neglecta</t>
+  </si>
+  <si>
+    <t>liana, yellowish when ripe.</t>
+  </si>
+  <si>
+    <t>Grow within the shrubs. Common. Growth with Embelia laeta.</t>
+  </si>
+  <si>
+    <t>CABINET_1_10</t>
+  </si>
+  <si>
+    <t>vegetative</t>
+  </si>
+  <si>
+    <t>JL0023</t>
+  </si>
+  <si>
+    <t>POACEAE</t>
+  </si>
+  <si>
+    <t>Poa</t>
+  </si>
+  <si>
+    <t>koenigii</t>
+  </si>
+  <si>
+    <t>FLORA OF HONG KONG</t>
+  </si>
+  <si>
+    <t>Herb, 40 to 60 cm tall, Spike with white hairs.</t>
+  </si>
+  <si>
+    <t>In steppe, open area.</t>
+  </si>
+  <si>
+    <t>JL0024</t>
+  </si>
+  <si>
+    <t>COMPOSITAE</t>
+  </si>
+  <si>
+    <t>Pluchea</t>
+  </si>
+  <si>
+    <t>sp.</t>
+  </si>
+  <si>
+    <t>herb, 50 - 70 cm tall. flowers purple.</t>
+  </si>
+  <si>
+    <t>On the sea shore, open, salty soil.</t>
+  </si>
+  <si>
+    <t>CABINET_1_15</t>
+  </si>
+  <si>
+    <t>JL0025</t>
+  </si>
+  <si>
+    <t>Panicum</t>
+  </si>
+  <si>
+    <t>maximum</t>
+  </si>
+  <si>
+    <t>Flowers green.</t>
+  </si>
+  <si>
+    <t>Along the road, common.</t>
+  </si>
+  <si>
+    <t>CABINET_43_10</t>
+  </si>
+  <si>
+    <t>JL0026</t>
+  </si>
+  <si>
+    <t>ACANTHACEAE</t>
+  </si>
+  <si>
+    <t>Justicia</t>
+  </si>
+  <si>
+    <t>ventricosa</t>
+  </si>
+  <si>
+    <t>herb, 1.2m tall.</t>
+  </si>
+  <si>
+    <t>Sea shore, along the sea shore, within the mangroves. Not common. Growth with Kandelia candel,Bruguiera gymnorrhiza,Avicennia marina,Excoecaria agallocha.</t>
+  </si>
+  <si>
+    <t>CABINET_45_6</t>
+  </si>
+  <si>
+    <t>JL0027</t>
+  </si>
+  <si>
+    <t>2014-9-4</t>
+  </si>
+  <si>
+    <t>LEGUMINOSAE</t>
+  </si>
+  <si>
+    <t>Canavalia</t>
+  </si>
+  <si>
+    <t>lineataw</t>
+  </si>
+  <si>
+    <t>Vine, flowers purple.</t>
+  </si>
+  <si>
+    <t>along the sea shore, among the mangroves. Not common. Growth with Kandelia candel,Bruguiera sp..</t>
+  </si>
+  <si>
+    <t>CABINET_53_11</t>
+  </si>
+  <si>
+    <t>JL0028</t>
+  </si>
+  <si>
+    <t>LENTIBULARIACEAE</t>
+  </si>
+  <si>
+    <t>Utricularia</t>
+  </si>
+  <si>
+    <t>biflorae</t>
+  </si>
+  <si>
+    <t>Aquatic plant, flowers yellow.</t>
+  </si>
+  <si>
+    <t>In flowing fresh water, open, sunny pool. Uncommon.</t>
+  </si>
+  <si>
+    <t>CABINET_40_16</t>
+  </si>
+  <si>
+    <t>JL0029</t>
+  </si>
+  <si>
+    <t>ORCHIDACEAE</t>
+  </si>
+  <si>
+    <t>Spiranthes</t>
+  </si>
+  <si>
+    <t>hongkongensis</t>
+  </si>
+  <si>
+    <t>herb, 15 to 20cm tall. Flowers white.</t>
+  </si>
+  <si>
+    <t>Along the trail in country park.</t>
+  </si>
+  <si>
+    <t>CABINET_40_7</t>
+  </si>
+  <si>
+    <t>JL0030</t>
+  </si>
+  <si>
+    <t>Geissaspis343434</t>
+  </si>
+  <si>
+    <t>cristata</t>
+  </si>
+  <si>
+    <t>papery leave blades, slightly hairy.</t>
+  </si>
+  <si>
+    <t>in very wet grassland. Near sea shore.</t>
+  </si>
+  <si>
+    <t>CABINET_34_2</t>
+  </si>
+  <si>
     <t>(Dennst.) Prain.</t>
-  </si>
-  <si>
-    <t>HONG KONG</t>
-  </si>
-  <si>
-    <t>New Territories</t>
-  </si>
-  <si>
-    <t>Sai Kung District</t>
-  </si>
-  <si>
-    <t>Yung Shue O</t>
-  </si>
-  <si>
-    <t>FLORA OF CHINA</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>Liana.</t>
-  </si>
-  <si>
-    <t>in dense forest.</t>
-  </si>
-  <si>
-    <t>CABINET_1_1</t>
-  </si>
-  <si>
-    <t>in herbarium</t>
-  </si>
-  <si>
-    <t>GPS</t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>50m</t>
-  </si>
-  <si>
-    <t>2015-02-04</t>
-  </si>
-  <si>
-    <t>JL0020</t>
-  </si>
-  <si>
-    <t>MALVACEAE</t>
-  </si>
-  <si>
-    <t>Swartzia</t>
-  </si>
-  <si>
-    <t>australis</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>S. Y. Hu &amp; Barretto</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wight &amp; Arn.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lour.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(Thunb.) DC.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wall.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jacq.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(Retz.) P. Beauv.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>L.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>(R. Br.) Miq.</t>
-  </si>
-  <si>
-    <t>herb, 10-15cm.</t>
-  </si>
-  <si>
-    <t>Sea shore, along the sea shore, near the mangroves. Grow in open areas.</t>
-  </si>
-  <si>
-    <t>CABINET_1_14</t>
-  </si>
-  <si>
-    <t>flowering</t>
-  </si>
-  <si>
-    <t>JL0021</t>
-  </si>
-  <si>
-    <t>COMBRETACEAE</t>
-  </si>
-  <si>
-    <t>Lumnitzera</t>
-  </si>
-  <si>
-    <t>racemosa</t>
-  </si>
-  <si>
-    <t>shrub, 2m tall. Flowers white.</t>
-  </si>
-  <si>
-    <t>Sea shore, along the sea shore, within the mangroves. Not common. Growth with Kandelia candel,Bruguiera gymnorrhiza,Avicennia marina.</t>
-  </si>
-  <si>
-    <t>CABINET_1_16</t>
-  </si>
-  <si>
-    <t>JL0022</t>
-  </si>
-  <si>
-    <t>2014-8-15</t>
-  </si>
-  <si>
-    <t>PASSIFLORACEAE</t>
-  </si>
-  <si>
-    <t>Cyclobalanosis</t>
-  </si>
-  <si>
-    <t>neglecta</t>
-  </si>
-  <si>
-    <t>L.</t>
-  </si>
-  <si>
-    <t>liana, yellowish when ripe.</t>
-  </si>
-  <si>
-    <t>Grow within the shrubs. Common. Growth with Embelia laeta.</t>
-  </si>
-  <si>
-    <t>CABINET_1_10</t>
-  </si>
-  <si>
-    <t>vegetative</t>
-  </si>
-  <si>
-    <t>JL0023</t>
-  </si>
-  <si>
-    <t>POACEAE</t>
-  </si>
-  <si>
-    <t>Poa</t>
-  </si>
-  <si>
-    <t>koenigii</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Retz.) P. Beauv. </t>
-  </si>
-  <si>
-    <t>FLORA OF HONG KONG</t>
-  </si>
-  <si>
-    <t>Herb, 40 to 60 cm tall, Spike with white hairs.</t>
-  </si>
-  <si>
-    <t>In steppe, open area.</t>
-  </si>
-  <si>
-    <t>JL0024</t>
-  </si>
-  <si>
-    <t>COMPOSITAE</t>
-  </si>
-  <si>
-    <t>Pluchea</t>
-  </si>
-  <si>
-    <t>sp.</t>
-  </si>
-  <si>
-    <t>herb, 50 - 70 cm tall. flowers purple.</t>
-  </si>
-  <si>
-    <t>On the sea shore, open, salty soil.</t>
-  </si>
-  <si>
-    <t>CABINET_1_15</t>
-  </si>
-  <si>
-    <t>JL0025</t>
-  </si>
-  <si>
-    <t>Panicum</t>
-  </si>
-  <si>
-    <t>maximum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jacq. </t>
-  </si>
-  <si>
-    <t>Flowers green.</t>
-  </si>
-  <si>
-    <t>Along the road, common.</t>
-  </si>
-  <si>
-    <t>CABINET_43_10</t>
-  </si>
-  <si>
-    <t>JL0026</t>
-  </si>
-  <si>
-    <t>ACANTHACEAE</t>
-  </si>
-  <si>
-    <t>Justicia</t>
-  </si>
-  <si>
-    <t>ventricosa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wall. </t>
-  </si>
-  <si>
-    <t>herb, 1.2m tall.</t>
-  </si>
-  <si>
-    <t>Sea shore, along the sea shore, within the mangroves. Not common. Growth with Kandelia candel,Bruguiera gymnorrhiza,Avicennia marina,Excoecaria agallocha.</t>
-  </si>
-  <si>
-    <t>CABINET_45_6</t>
-  </si>
-  <si>
-    <t>JL0027</t>
-  </si>
-  <si>
-    <t>2014-9-4</t>
-  </si>
-  <si>
-    <t>LEGUMINOSAE</t>
-  </si>
-  <si>
-    <t>Canavalia</t>
-  </si>
-  <si>
-    <t>lineataw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Thunb.) DC. </t>
-  </si>
-  <si>
-    <t>Vine, flowers purple.</t>
-  </si>
-  <si>
-    <t>along the sea shore, among the mangroves. Not common. Growth with Kandelia candel,Bruguiera sp..</t>
-  </si>
-  <si>
-    <t>CABINET_53_11</t>
-  </si>
-  <si>
-    <t>JL0028</t>
-  </si>
-  <si>
-    <t>LENTIBULARIACEAE</t>
-  </si>
-  <si>
-    <t>Utricularia</t>
-  </si>
-  <si>
-    <t>biflorae</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lour. </t>
-  </si>
-  <si>
-    <t>Aquatic plant, flowers yellow.</t>
-  </si>
-  <si>
-    <t>In flowing fresh water, open, sunny pool. Uncommon.</t>
-  </si>
-  <si>
-    <t>CABINET_40_16</t>
-  </si>
-  <si>
-    <t>JL0029</t>
-  </si>
-  <si>
-    <t>ORCHIDACEAE</t>
-  </si>
-  <si>
-    <t>Spiranthes</t>
-  </si>
-  <si>
-    <t>hongkongensis</t>
-  </si>
-  <si>
-    <t>S. Y. Hu &amp; Barretto</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>var.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>stellaria</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>De Boiss</t>
-  </si>
-  <si>
-    <t>herb, 15 to 20cm tall. Flowers white.</t>
-  </si>
-  <si>
-    <t>Along the trail in country park.</t>
-  </si>
-  <si>
-    <t>CABINET_40_7</t>
-  </si>
-  <si>
-    <t>JL0030</t>
-  </si>
-  <si>
-    <t>Geissaspis343434</t>
-  </si>
-  <si>
-    <t>cristata</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wight &amp; Arn. </t>
-  </si>
-  <si>
-    <t>papery leave blades, slightly hairy.</t>
-  </si>
-  <si>
-    <t>in very wet grassland. Near sea shore.</t>
-  </si>
-  <si>
-    <t>CABINET_34_2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -546,42 +562,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Currency[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Percent" xfId="3" builtinId="5"/>
-    <cellStyle name="Currency" xfId="4" builtinId="4"/>
-    <cellStyle name="Comma[0]" xfId="5" builtinId="6"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -880,6 +886,7 @@
           </a:gdLst>
           <a:ahLst/>
           <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
           <a:pathLst>
             <a:path w="21600" h="21600"/>
           </a:pathLst>
@@ -912,28 +919,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AO1" workbookViewId="0">
-      <selection activeCell="AV14" sqref="AV14"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="12.55"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="10" width="9.23076923076923" style="1"/>
-    <col min="11" max="11" width="9.56410256410256" style="1"/>
-    <col min="12" max="43" width="9.23076923076923" style="1"/>
-    <col min="44" max="44" width="16.3162393162393" style="1" customWidth="1"/>
-    <col min="45" max="45" width="9.56410256410256" style="1"/>
-    <col min="46" max="46" width="9.23076923076923" style="1"/>
-    <col min="47" max="47" width="14.1623931623932" style="1" customWidth="1"/>
-    <col min="48" max="48" width="9.56410256410256" style="1"/>
-    <col min="49" max="16384" width="9.23076923076923" style="1"/>
+    <col min="1" max="10" width="9.21875" style="1"/>
+    <col min="11" max="11" width="9.5546875" style="1"/>
+    <col min="12" max="15" width="9.21875" style="1"/>
+    <col min="16" max="16" width="30.44140625" style="1" customWidth="1"/>
+    <col min="17" max="43" width="9.21875" style="1"/>
+    <col min="44" max="44" width="16.33203125" style="1" customWidth="1"/>
+    <col min="45" max="45" width="9.5546875" style="1"/>
+    <col min="46" max="46" width="9.21875" style="1"/>
+    <col min="47" max="47" width="14.109375" style="1" customWidth="1"/>
+    <col min="48" max="48" width="9.5546875" style="1"/>
+    <col min="49" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1079,7 +1087,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="2:48">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>48</v>
       </c>
@@ -1113,23 +1121,23 @@
       <c r="O2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="P2" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="AA2" s="1">
         <v>22</v>
@@ -1141,7 +1149,7 @@
         <v>45</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AE2" s="1">
         <v>114</v>
@@ -1153,46 +1161,46 @@
         <v>11</v>
       </c>
       <c r="AH2" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AI2" s="1">
         <v>2</v>
       </c>
       <c r="AJ2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AK2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AK2" s="1" t="s">
+      <c r="AL2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AL2" s="1" t="s">
+      <c r="AM2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AM2" s="1" t="s">
+      <c r="AN2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AN2" s="1" t="s">
+      <c r="AO2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AO2" s="1" t="s">
+      <c r="AP2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AP2" s="1" t="s">
+      <c r="AR2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AS2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AR2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS2" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="AU2" s="1" t="s">
         <v>52</v>
       </c>
       <c r="AV2" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
-    <row r="3" spans="2:48">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>48</v>
       </c>
@@ -1212,37 +1220,37 @@
         <v>52</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>54</v>
       </c>
       <c r="M3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>78</v>
+      <c r="P3" s="2" t="s">
+        <v>161</v>
       </c>
       <c r="T3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="U3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="W3" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="Z3" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="AA3" s="1">
         <v>22</v>
@@ -1254,7 +1262,7 @@
         <v>36</v>
       </c>
       <c r="AD3" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AE3" s="1">
         <v>114</v>
@@ -1266,46 +1274,46 @@
         <v>16</v>
       </c>
       <c r="AH3" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AI3" s="1">
         <v>1</v>
       </c>
       <c r="AJ3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AK3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AL3" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AK3" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AL3" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="AM3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN3" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AN3" s="1" t="s">
+      <c r="AO3" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AO3" s="1" t="s">
+      <c r="AP3" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AP3" s="1" t="s">
+      <c r="AR3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AS3" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AR3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS3" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="AU3" s="1" t="s">
         <v>52</v>
       </c>
       <c r="AV3" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
-    <row r="4" spans="2:48">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>48</v>
       </c>
@@ -1316,7 +1324,7 @@
         <v>49</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>51</v>
@@ -1325,34 +1333,34 @@
         <v>52</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>54</v>
       </c>
       <c r="M4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="N4" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="T4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="U4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="V4" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="W4" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="W4" s="1" t="s">
+      <c r="Z4" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="Z4" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="AA4" s="1">
         <v>22</v>
@@ -1364,7 +1372,7 @@
         <v>35</v>
       </c>
       <c r="AD4" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AE4" s="1">
         <v>114</v>
@@ -1376,46 +1384,46 @@
         <v>17</v>
       </c>
       <c r="AH4" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AI4" s="1">
         <v>1</v>
       </c>
       <c r="AJ4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AK4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AL4" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="AK4" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AL4" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="AM4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN4" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AN4" s="1" t="s">
+      <c r="AO4" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AO4" s="1" t="s">
+      <c r="AP4" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AP4" s="1" t="s">
+      <c r="AR4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AS4" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AR4" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS4" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="AU4" s="1" t="s">
         <v>52</v>
       </c>
       <c r="AV4" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
-    <row r="5" spans="2:48">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>48</v>
       </c>
@@ -1426,7 +1434,7 @@
         <v>49</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>51</v>
@@ -1435,37 +1443,37 @@
         <v>52</v>
       </c>
       <c r="J5" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="O5" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="N5" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>95</v>
+      <c r="P5" s="2" t="s">
+        <v>160</v>
       </c>
       <c r="T5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="U5" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="U5" s="1" t="s">
+      <c r="V5" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="V5" s="1" t="s">
+      <c r="W5" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="W5" s="1" t="s">
+      <c r="Z5" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="Z5" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="AA5" s="1">
         <v>22</v>
@@ -1477,7 +1485,7 @@
         <v>45</v>
       </c>
       <c r="AD5" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AE5" s="1">
         <v>114</v>
@@ -1489,46 +1497,46 @@
         <v>19</v>
       </c>
       <c r="AH5" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AI5" s="1">
         <v>1</v>
       </c>
       <c r="AJ5" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="AK5" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="AL5" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="AM5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN5" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AN5" s="1" t="s">
+      <c r="AO5" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AO5" s="1" t="s">
+      <c r="AP5" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AP5" s="1" t="s">
+      <c r="AR5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AS5" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AR5" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS5" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="AU5" s="1" t="s">
         <v>52</v>
       </c>
       <c r="AV5" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
-    <row r="6" spans="2:48">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>48</v>
       </c>
@@ -1539,7 +1547,7 @@
         <v>49</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>51</v>
@@ -1548,37 +1556,37 @@
         <v>52</v>
       </c>
       <c r="J6" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="O6" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="M6" s="1" t="s">
+      <c r="P6" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z6" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="V6" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="W6" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z6" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="AA6" s="1">
         <v>22</v>
@@ -1590,7 +1598,7 @@
         <v>43</v>
       </c>
       <c r="AD6" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AE6" s="1">
         <v>114</v>
@@ -1602,46 +1610,46 @@
         <v>23</v>
       </c>
       <c r="AH6" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AI6" s="1">
         <v>1</v>
       </c>
       <c r="AJ6" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="AK6" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="AL6" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="AM6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN6" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AN6" s="1" t="s">
+      <c r="AO6" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AO6" s="1" t="s">
+      <c r="AP6" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AP6" s="1" t="s">
+      <c r="AR6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AS6" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AR6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS6" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="AU6" s="1" t="s">
         <v>52</v>
       </c>
       <c r="AV6" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
-    <row r="7" spans="2:48">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>48</v>
       </c>
@@ -1652,7 +1660,7 @@
         <v>49</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>51</v>
@@ -1661,34 +1669,34 @@
         <v>52</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="T7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="U7" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="U7" s="1" t="s">
+      <c r="V7" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="V7" s="1" t="s">
+      <c r="W7" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="W7" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="Z7" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="AA7" s="1">
         <v>22</v>
@@ -1700,7 +1708,7 @@
         <v>45</v>
       </c>
       <c r="AD7" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AE7" s="1">
         <v>114</v>
@@ -1712,46 +1720,46 @@
         <v>19</v>
       </c>
       <c r="AH7" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AI7" s="1">
         <v>1</v>
       </c>
       <c r="AJ7" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="AK7" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="AL7" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="AM7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN7" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AN7" s="1" t="s">
+      <c r="AO7" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AO7" s="1" t="s">
+      <c r="AP7" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AP7" s="1" t="s">
+      <c r="AR7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AS7" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AR7" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS7" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="AU7" s="1" t="s">
         <v>52</v>
       </c>
       <c r="AV7" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
-    <row r="8" spans="2:48">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>48</v>
       </c>
@@ -1762,7 +1770,7 @@
         <v>49</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>51</v>
@@ -1771,37 +1779,37 @@
         <v>52</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="M8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z8" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="T8" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="U8" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="V8" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="W8" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z8" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="AA8" s="1">
         <v>22</v>
@@ -1813,7 +1821,7 @@
         <v>45</v>
       </c>
       <c r="AD8" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AE8" s="1">
         <v>114</v>
@@ -1825,46 +1833,46 @@
         <v>19</v>
       </c>
       <c r="AH8" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AI8" s="1">
         <v>1</v>
       </c>
       <c r="AJ8" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="AK8" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="AL8" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="AM8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN8" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AN8" s="1" t="s">
+      <c r="AO8" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AO8" s="1" t="s">
+      <c r="AP8" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AP8" s="1" t="s">
+      <c r="AR8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AS8" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AR8" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS8" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="AU8" s="1" t="s">
         <v>52</v>
       </c>
       <c r="AV8" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
-    <row r="9" spans="2:48">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>48</v>
       </c>
@@ -1875,7 +1883,7 @@
         <v>49</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>51</v>
@@ -1884,37 +1892,37 @@
         <v>52</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>157</v>
       </c>
       <c r="T9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="U9" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="U9" s="1" t="s">
+      <c r="V9" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="V9" s="1" t="s">
+      <c r="W9" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="W9" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="Z9" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="AA9" s="1">
         <v>22</v>
@@ -1926,7 +1934,7 @@
         <v>45</v>
       </c>
       <c r="AD9" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AE9" s="1">
         <v>114</v>
@@ -1938,46 +1946,46 @@
         <v>19</v>
       </c>
       <c r="AH9" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AI9" s="1">
         <v>1</v>
       </c>
       <c r="AJ9" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="AK9" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="AL9" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="AM9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN9" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AN9" s="1" t="s">
+      <c r="AO9" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AO9" s="1" t="s">
+      <c r="AP9" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AP9" s="1" t="s">
+      <c r="AR9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AS9" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AR9" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS9" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="AU9" s="1" t="s">
         <v>52</v>
       </c>
       <c r="AV9" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
-    <row r="10" spans="2:48">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>48</v>
       </c>
@@ -1988,7 +1996,7 @@
         <v>49</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>51</v>
@@ -1997,37 +2005,37 @@
         <v>52</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>135</v>
+        <v>128</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>156</v>
       </c>
       <c r="T10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="U10" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="U10" s="1" t="s">
+      <c r="V10" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="V10" s="1" t="s">
+      <c r="W10" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="W10" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="Z10" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="AA10" s="1">
         <v>22</v>
@@ -2039,7 +2047,7 @@
         <v>45</v>
       </c>
       <c r="AD10" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AE10" s="1">
         <v>114</v>
@@ -2051,46 +2059,46 @@
         <v>19</v>
       </c>
       <c r="AH10" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AI10" s="1">
         <v>1</v>
       </c>
       <c r="AJ10" s="1" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="AK10" s="1" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="AL10" s="1" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="AM10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN10" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AN10" s="1" t="s">
+      <c r="AO10" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AO10" s="1" t="s">
+      <c r="AP10" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AP10" s="1" t="s">
+      <c r="AR10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AS10" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AR10" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS10" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="AU10" s="1" t="s">
         <v>52</v>
       </c>
       <c r="AV10" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
-    <row r="11" spans="2:48">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>48</v>
       </c>
@@ -2101,7 +2109,7 @@
         <v>49</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>51</v>
@@ -2110,37 +2118,37 @@
         <v>52</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>143</v>
+        <v>135</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>155</v>
       </c>
       <c r="T11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="U11" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="U11" s="1" t="s">
+      <c r="V11" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="V11" s="1" t="s">
+      <c r="W11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="W11" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="Z11" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="AA11" s="1">
         <v>22</v>
@@ -2152,7 +2160,7 @@
         <v>45</v>
       </c>
       <c r="AD11" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AE11" s="1">
         <v>114</v>
@@ -2164,46 +2172,46 @@
         <v>19</v>
       </c>
       <c r="AH11" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AI11" s="1">
         <v>1</v>
       </c>
       <c r="AJ11" s="1" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="AK11" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="AL11" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="AM11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN11" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AN11" s="1" t="s">
+      <c r="AO11" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AO11" s="1" t="s">
+      <c r="AP11" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AP11" s="1" t="s">
+      <c r="AR11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AS11" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AR11" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS11" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="AU11" s="1" t="s">
         <v>52</v>
       </c>
       <c r="AV11" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
-    <row r="12" spans="2:48">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>48</v>
       </c>
@@ -2214,7 +2222,7 @@
         <v>49</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>51</v>
@@ -2223,46 +2231,46 @@
         <v>52</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="R12" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="P12" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="S12" s="1" t="s">
-        <v>154</v>
+      <c r="Q12" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="T12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="U12" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="U12" s="1" t="s">
+      <c r="V12" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="V12" s="1" t="s">
+      <c r="W12" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="W12" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="Z12" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="AA12" s="1">
         <v>22</v>
@@ -2274,7 +2282,7 @@
         <v>45</v>
       </c>
       <c r="AD12" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AE12" s="1">
         <v>114</v>
@@ -2286,46 +2294,46 @@
         <v>19</v>
       </c>
       <c r="AH12" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AI12" s="1">
         <v>1</v>
       </c>
       <c r="AJ12" s="1" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="AK12" s="1" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="AL12" s="1" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="AM12" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN12" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AN12" s="1" t="s">
+      <c r="AO12" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AO12" s="1" t="s">
+      <c r="AP12" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AP12" s="1" t="s">
+      <c r="AR12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AS12" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AR12" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS12" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="AU12" s="1" t="s">
         <v>52</v>
       </c>
       <c r="AV12" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
-    <row r="13" spans="2:48">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>48</v>
       </c>
@@ -2336,7 +2344,7 @@
         <v>49</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>51</v>
@@ -2345,37 +2353,37 @@
         <v>52</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>161</v>
+        <v>148</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>154</v>
       </c>
       <c r="T13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="U13" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="U13" s="1" t="s">
+      <c r="V13" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="V13" s="1" t="s">
+      <c r="W13" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="W13" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="Z13" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="AA13" s="1">
         <v>22</v>
@@ -2387,7 +2395,7 @@
         <v>45</v>
       </c>
       <c r="AD13" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AE13" s="1">
         <v>114</v>
@@ -2399,47 +2407,47 @@
         <v>19</v>
       </c>
       <c r="AH13" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AI13" s="1">
         <v>1</v>
       </c>
       <c r="AJ13" s="1" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="AK13" s="1" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="AL13" s="1" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="AM13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN13" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AN13" s="1" t="s">
+      <c r="AO13" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AO13" s="1" t="s">
+      <c r="AP13" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AP13" s="1" t="s">
+      <c r="AR13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AS13" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AR13" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS13" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="AU13" s="1" t="s">
         <v>52</v>
       </c>
       <c r="AV13" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
-  <headerFooter/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
automatically parse and fill the taxonomic fields
</commit_message>
<xml_diff>
--- a/inst/extdata/DARWIN_CORE_HERBARIUM_RECORDS_TEMPLATE.xlsx
+++ b/inst/extdata/DARWIN_CORE_HERBARIUM_RECORDS_TEMPLATE.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="177">
   <si>
     <t>GLOBAL_UNIQUE_IDENTIFIER</t>
   </si>
@@ -522,13 +522,52 @@
   <si>
     <t>De Boiss</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>华润楠</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>阔苞菊</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>榄李</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>翅果蓼属</t>
+  </si>
+  <si>
+    <t>翅果蓼屬</t>
+  </si>
+  <si>
+    <t>翅果蓼</t>
+  </si>
+  <si>
+    <t>多瓣核果茶属</t>
+  </si>
+  <si>
+    <t>多瓣核果茶屬</t>
+  </si>
+  <si>
+    <t>多瓣核果茶</t>
+  </si>
+  <si>
+    <t>拟楼斗菜属</t>
+  </si>
+  <si>
+    <t>擬樓鬥菜屬</t>
+  </si>
+  <si>
+    <t>乳突拟耧斗菜</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -543,6 +582,12 @@
       <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="FangSong"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -567,7 +612,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -575,6 +620,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -920,17 +968,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AV13"/>
+  <dimension ref="A1:AV16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="10" width="9.21875" style="1"/>
     <col min="11" max="11" width="9.5546875" style="1"/>
-    <col min="12" max="15" width="9.21875" style="1"/>
+    <col min="12" max="12" width="17.21875" style="1" customWidth="1"/>
+    <col min="13" max="15" width="9.21875" style="1"/>
     <col min="16" max="16" width="30.44140625" style="1" customWidth="1"/>
     <col min="17" max="43" width="9.21875" style="1"/>
     <col min="44" max="44" width="16.33203125" style="1" customWidth="1"/>
@@ -1112,6 +1161,9 @@
       <c r="K2" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="L2" s="3" t="s">
+        <v>165</v>
+      </c>
       <c r="M2" s="1" t="s">
         <v>55</v>
       </c>
@@ -1225,6 +1277,9 @@
       <c r="K3" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="L3" s="3" t="s">
+        <v>166</v>
+      </c>
       <c r="M3" s="1" t="s">
         <v>74</v>
       </c>
@@ -1338,6 +1393,9 @@
       <c r="K4" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="L4" s="3" t="s">
+        <v>167</v>
+      </c>
       <c r="M4" s="1" t="s">
         <v>82</v>
       </c>
@@ -1448,6 +1506,9 @@
       <c r="K5" s="1" t="s">
         <v>89</v>
       </c>
+      <c r="L5" s="3" t="s">
+        <v>168</v>
+      </c>
       <c r="M5" s="1" t="s">
         <v>90</v>
       </c>
@@ -1561,6 +1622,9 @@
       <c r="K6" s="1" t="s">
         <v>89</v>
       </c>
+      <c r="L6" s="3" t="s">
+        <v>169</v>
+      </c>
       <c r="M6" s="1" t="s">
         <v>98</v>
       </c>
@@ -1674,6 +1738,9 @@
       <c r="K7" s="1" t="s">
         <v>89</v>
       </c>
+      <c r="L7" s="3" t="s">
+        <v>170</v>
+      </c>
       <c r="M7" s="1" t="s">
         <v>105</v>
       </c>
@@ -1784,6 +1851,9 @@
       <c r="K8" s="1" t="s">
         <v>89</v>
       </c>
+      <c r="L8" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="M8" s="1" t="s">
         <v>98</v>
       </c>
@@ -1897,6 +1967,9 @@
       <c r="K9" s="1" t="s">
         <v>89</v>
       </c>
+      <c r="L9" s="3" t="s">
+        <v>172</v>
+      </c>
       <c r="M9" s="1" t="s">
         <v>118</v>
       </c>
@@ -2010,6 +2083,9 @@
       <c r="K10" s="1" t="s">
         <v>125</v>
       </c>
+      <c r="L10" s="3" t="s">
+        <v>173</v>
+      </c>
       <c r="M10" s="1" t="s">
         <v>126</v>
       </c>
@@ -2123,6 +2199,9 @@
       <c r="K11" s="1" t="s">
         <v>125</v>
       </c>
+      <c r="L11" s="3" t="s">
+        <v>174</v>
+      </c>
       <c r="M11" s="1" t="s">
         <v>133</v>
       </c>
@@ -2236,6 +2315,9 @@
       <c r="K12" s="1" t="s">
         <v>125</v>
       </c>
+      <c r="L12" s="3" t="s">
+        <v>175</v>
+      </c>
       <c r="M12" s="1" t="s">
         <v>140</v>
       </c>
@@ -2358,6 +2440,9 @@
       <c r="K13" s="1" t="s">
         <v>125</v>
       </c>
+      <c r="L13" s="3" t="s">
+        <v>176</v>
+      </c>
       <c r="M13" s="1" t="s">
         <v>126</v>
       </c>
@@ -2445,6 +2530,15 @@
       <c r="AV13" s="1" t="s">
         <v>72</v>
       </c>
+    </row>
+    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="L15" s="3"/>
+    </row>
+    <row r="16" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="L16" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>